<commit_message>
Rearranged pin location settings
</commit_message>
<xml_diff>
--- a/Operations Manager/Test Utilities/LBCB Pin Positions.xlsx
+++ b/Operations Manager/Test Utilities/LBCB Pin Positions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t xml:space="preserve">Small </t>
   </si>
@@ -139,15 +139,58 @@
   </si>
   <si>
     <t>p36</t>
+  </si>
+  <si>
+    <t>Conventions</t>
+  </si>
+  <si>
+    <t>b or p</t>
+  </si>
+  <si>
+    <t>base or patform pin position</t>
+  </si>
+  <si>
+    <r>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AB</t>
+    </r>
+  </si>
+  <si>
+    <t>Examples</t>
+  </si>
+  <si>
+    <t>Base pin, X1</t>
+  </si>
+  <si>
+    <t>Platform pin, Z3</t>
+  </si>
+  <si>
+    <t>A is the dof x,y ,or z .  B is the actuator number X1, X2, Y1, Z1, Z2, Z3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -174,8 +217,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -620,7 +666,7 @@
         <v>-1.9690000000000001</v>
       </c>
       <c r="G4">
-        <v>1.9690000000000001</v>
+        <v>-1.9690000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -686,10 +732,10 @@
         <v>24</v>
       </c>
       <c r="F7">
-        <v>4.8</v>
+        <v>-4.8</v>
       </c>
       <c r="G7">
-        <v>4.8</v>
+        <v>-4.8</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -755,10 +801,10 @@
         <v>-24</v>
       </c>
       <c r="F10">
-        <v>-1.9690000000000001</v>
+        <v>1.9690000000000001</v>
       </c>
       <c r="G10">
-        <v>-1.9690000000000001</v>
+        <v>1.9690000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -824,10 +870,10 @@
         <v>-24</v>
       </c>
       <c r="F13">
-        <v>-4.8</v>
+        <v>4.8</v>
       </c>
       <c r="G13">
-        <v>-4.8</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1412,13 +1458,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="48.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>